<commit_message>
fix bugs; add changes;
</commit_message>
<xml_diff>
--- a/templates/Test Data.xlsx
+++ b/templates/Test Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Unit-PC\OneDrive\Documents\work\CVS\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chironitcom.sharepoint.com/sites/Demo/cvs/SiteAssets/DRProcessAutomationSolution/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F89E0D-41A9-46FD-BA2C-29C23C4F63E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{0B1532E5-6BD8-4381-92F7-1D0452124977}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16310" windowWidth="29020" windowHeight="15820" xr2:uid="{0CD1BEDA-7486-4720-A476-202218AA02F8}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>Larry Lavanaway</t>
   </si>
   <si>
-    <t>David Antolovich</t>
-  </si>
-  <si>
     <t>APIGEE Edge API Management</t>
   </si>
   <si>
@@ -192,7 +189,10 @@
     <t>&lt; 7 Days</t>
   </si>
   <si>
-    <t>Alex Pashkevych</t>
+    <t>Yaroslav Masyuk</t>
+  </si>
+  <si>
+    <t>Alex Pashkevych; Yaroslav Masyuk</t>
   </si>
 </sst>
 </file>
@@ -804,16 +804,16 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -834,7 +834,7 @@
         <v>ENROLLMENT INTAKE</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>15</v>
@@ -843,7 +843,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -856,22 +856,22 @@
         <v>44212</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -884,22 +884,22 @@
         <v>44213</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>41</v>
-      </c>
       <c r="G5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -912,22 +912,22 @@
         <v>44214</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -940,22 +940,22 @@
         <v>44215</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="G7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -968,22 +968,22 @@
         <v>44216</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -999,19 +999,19 @@
         <v>12</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="G9" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -1024,22 +1024,22 @@
         <v>44218</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -1055,19 +1055,19 @@
         <v>12</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="G11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -1080,22 +1080,22 @@
         <v>44220</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1109,6 +1109,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F9C2C2B2406125409A3F17BA3F7FD346" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f10644555745b267360e20d28f7b5fca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="91fec23a-896d-4a11-b055-6e622c7ebd3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24e92bd2515386aafdd8dc0691a59344" ns2:_="">
     <xsd:import namespace="91fec23a-896d-4a11-b055-6e622c7ebd3e"/>
@@ -1258,29 +1273,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC34A2CA-789A-48E7-84D9-942FFDB7913B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08672846-9B6E-454E-8826-DD1718B11D4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33E1D047-EC85-4DF8-8DBE-8C0463338BAA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33E1D047-EC85-4DF8-8DBE-8C0463338BAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08672846-9B6E-454E-8826-DD1718B11D4C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC34A2CA-789A-48E7-84D9-942FFDB7913B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="91fec23a-896d-4a11-b055-6e622c7ebd3e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>